<commit_message>
Modifica db, tuple e funzioni per parametri filippine
</commit_message>
<xml_diff>
--- a/resources/filippine.xlsx
+++ b/resources/filippine.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>3aU2d</t>
   </si>
@@ -69,12 +69,6 @@
     <t>phimax</t>
   </si>
   <si>
-    <t>cmin</t>
-  </si>
-  <si>
-    <t>cmax</t>
-  </si>
-  <si>
     <t>UCS_matrix</t>
   </si>
   <si>
@@ -96,60 +90,18 @@
     <t>D</t>
   </si>
   <si>
-    <t>ei_min</t>
-  </si>
-  <si>
-    <t>ei_max</t>
-  </si>
-  <si>
-    <t>phi_nom</t>
-  </si>
-  <si>
-    <t>ei_nom</t>
-  </si>
-  <si>
-    <t>c_nom</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>g_med</t>
   </si>
   <si>
     <t>g_stddev</t>
   </si>
   <si>
-    <t>sigma_ci_avg</t>
-  </si>
-  <si>
-    <t>sigma_ci_stdev</t>
-  </si>
-  <si>
-    <t>mi_med</t>
-  </si>
-  <si>
-    <t>mi_stdev</t>
-  </si>
-  <si>
     <t>ei_med</t>
   </si>
   <si>
     <t>ei_stdev</t>
   </si>
   <si>
-    <t>cai_med</t>
-  </si>
-  <si>
-    <t>cai_stdev</t>
-  </si>
-  <si>
-    <t>gsi_med</t>
-  </si>
-  <si>
-    <t>gsi_stdev</t>
-  </si>
-  <si>
     <t>rmr_med</t>
   </si>
   <si>
@@ -159,12 +111,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>sigma_ti_min</t>
-  </si>
-  <si>
-    <t>sigma_ti_max</t>
-  </si>
-  <si>
     <t>k0_min</t>
   </si>
   <si>
@@ -174,7 +120,22 @@
     <t>Id</t>
   </si>
   <si>
-    <t>rmr</t>
+    <t>Modulo deformazione</t>
+  </si>
+  <si>
+    <t>Qualità ammasso</t>
+  </si>
+  <si>
+    <t>w_inflow_min</t>
+  </si>
+  <si>
+    <t>w_inflow_max</t>
+  </si>
+  <si>
+    <t>c_stdev</t>
+  </si>
+  <si>
+    <t>c_med</t>
   </si>
 </sst>
 </file>
@@ -205,32 +166,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="22"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -241,8 +187,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -523,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,128 +480,74 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="5" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5703125" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" customWidth="1"/>
     <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="3" t="s">
+    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>29</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -664,58 +556,70 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
       <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V3" t="s">
         <v>13</v>
       </c>
-      <c r="O3" t="s">
+      <c r="W3" t="s">
         <v>14</v>
       </c>
-      <c r="P3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3" t="s">
-        <v>42</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>15</v>
       </c>
-      <c r="X3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -733,52 +637,65 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <f>2.75*0.8+2.1*0.2</f>
+        <v>2.62</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>23</v>
+      </c>
+      <c r="J4">
+        <v>35</v>
+      </c>
+      <c r="K4">
         <v>300</v>
       </c>
-      <c r="I4">
-        <v>300</v>
-      </c>
-      <c r="J4">
-        <v>300</v>
-      </c>
-      <c r="K4">
-        <v>23</v>
-      </c>
       <c r="L4">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="N4">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="P4">
-        <v>120</v>
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0.5</v>
       </c>
       <c r="S4">
-        <v>50</v>
-      </c>
-      <c r="U4" t="s">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="T4">
+        <v>10</v>
+      </c>
+      <c r="U4">
+        <v>25</v>
+      </c>
+      <c r="V4">
+        <v>4</v>
       </c>
       <c r="W4">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="X4">
-        <v>100</v>
-      </c>
-      <c r="Y4">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -796,52 +713,65 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G6" si="1">2.75*0.8+2.1*0.2</f>
+        <v>2.62</v>
       </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>32</v>
+      </c>
+      <c r="K5">
         <v>380</v>
       </c>
-      <c r="I5">
-        <v>380</v>
-      </c>
-      <c r="J5">
-        <v>380</v>
-      </c>
-      <c r="K5">
-        <v>22</v>
-      </c>
       <c r="L5">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>27</v>
+        <v>150</v>
       </c>
       <c r="N5">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="P5">
-        <v>150</v>
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>0.5</v>
       </c>
       <c r="S5">
-        <v>50</v>
-      </c>
-      <c r="U5" t="s">
-        <v>3</v>
+        <v>1.5</v>
+      </c>
+      <c r="T5">
+        <v>10</v>
+      </c>
+      <c r="U5">
+        <v>25</v>
+      </c>
+      <c r="V5">
+        <v>4</v>
       </c>
       <c r="W5">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="X5">
-        <v>100</v>
-      </c>
-      <c r="Y5">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -852,59 +782,72 @@
         <v>1090</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" ref="D6:D15" si="1">C6-B6</f>
+        <f t="shared" ref="D6:D15" si="2">C6-B6</f>
         <v>580</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>2.62</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
         <v>21</v>
       </c>
-      <c r="H6" s="2">
+      <c r="J6" s="2">
+        <v>30</v>
+      </c>
+      <c r="K6" s="2">
         <v>400</v>
       </c>
-      <c r="I6" s="2">
-        <v>400</v>
-      </c>
-      <c r="J6" s="2">
-        <v>400</v>
-      </c>
-      <c r="K6" s="2">
-        <v>21</v>
-      </c>
-      <c r="L6" s="2">
-        <v>30</v>
+      <c r="L6">
+        <v>0</v>
       </c>
       <c r="M6" s="2">
+        <v>180</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>50</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>0.5</v>
+      </c>
+      <c r="S6">
+        <v>1.5</v>
+      </c>
+      <c r="T6">
+        <v>10</v>
+      </c>
+      <c r="U6">
         <v>25</v>
       </c>
-      <c r="N6" s="2">
-        <v>180</v>
-      </c>
-      <c r="O6" s="2">
-        <v>180</v>
-      </c>
-      <c r="P6" s="2">
-        <v>180</v>
-      </c>
-      <c r="S6">
-        <v>50</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>1</v>
+      <c r="V6" s="2">
+        <v>6</v>
       </c>
       <c r="W6" s="2">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="X6" s="2">
-        <v>100</v>
-      </c>
-      <c r="Y6" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -915,59 +858,71 @@
         <v>1690</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>600</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>21</v>
       </c>
-      <c r="H7">
+      <c r="J7">
+        <v>30</v>
+      </c>
+      <c r="K7">
         <v>420</v>
       </c>
-      <c r="I7">
-        <v>420</v>
-      </c>
-      <c r="J7">
-        <v>420</v>
-      </c>
-      <c r="K7">
-        <v>21</v>
-      </c>
       <c r="L7">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M7">
+        <v>180</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>50</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>0.5</v>
+      </c>
+      <c r="S7">
+        <v>1.5</v>
+      </c>
+      <c r="T7">
+        <v>10</v>
+      </c>
+      <c r="U7">
         <v>25</v>
       </c>
-      <c r="N7">
-        <v>180</v>
-      </c>
-      <c r="O7">
-        <v>180</v>
-      </c>
-      <c r="P7">
-        <v>180</v>
-      </c>
-      <c r="S7">
-        <v>50</v>
-      </c>
-      <c r="U7" t="s">
-        <v>2</v>
+      <c r="V7">
+        <v>8</v>
       </c>
       <c r="W7">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="X7">
         <v>0</v>
       </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -978,59 +933,72 @@
         <v>2550</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>860</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8">
+        <f>2.75*0.8+2.1*0.2</f>
+        <v>2.62</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>21</v>
       </c>
-      <c r="H8">
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8">
         <v>400</v>
       </c>
-      <c r="I8">
-        <v>400</v>
-      </c>
-      <c r="J8">
-        <v>400</v>
-      </c>
-      <c r="K8">
-        <v>21</v>
-      </c>
       <c r="L8">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M8">
+        <v>180</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>50</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0.5</v>
+      </c>
+      <c r="S8">
+        <v>1.5</v>
+      </c>
+      <c r="T8">
+        <v>10</v>
+      </c>
+      <c r="U8">
         <v>25</v>
       </c>
-      <c r="N8">
-        <v>180</v>
-      </c>
-      <c r="O8">
-        <v>180</v>
-      </c>
-      <c r="P8">
-        <v>180</v>
-      </c>
-      <c r="S8">
-        <v>50</v>
-      </c>
-      <c r="U8" t="s">
-        <v>1</v>
+      <c r="V8">
+        <v>6</v>
       </c>
       <c r="W8">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="X8">
-        <v>100</v>
-      </c>
-      <c r="Y8">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1041,59 +1009,71 @@
         <v>3140</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>590</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>21</v>
       </c>
-      <c r="H9">
+      <c r="J9">
+        <v>30</v>
+      </c>
+      <c r="K9">
         <v>420</v>
       </c>
-      <c r="I9">
-        <v>420</v>
-      </c>
-      <c r="J9">
-        <v>420</v>
-      </c>
-      <c r="K9">
-        <v>21</v>
-      </c>
       <c r="L9">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>25</v>
+        <v>180</v>
       </c>
       <c r="N9">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>180</v>
+        <v>50</v>
       </c>
       <c r="P9">
-        <v>180</v>
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9">
+        <v>0.5</v>
       </c>
       <c r="S9">
-        <v>50</v>
-      </c>
-      <c r="U9" t="s">
-        <v>2</v>
+        <v>1.5</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>10</v>
+      </c>
+      <c r="V9">
+        <v>8</v>
       </c>
       <c r="W9">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="X9">
         <v>0</v>
       </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1104,59 +1084,72 @@
         <v>3660</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>520</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10">
+        <v>19</v>
+      </c>
+      <c r="G10">
+        <f>2.75*0.8+2.1*0.2</f>
+        <v>2.62</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>22</v>
+      </c>
+      <c r="J10">
+        <v>32</v>
+      </c>
+      <c r="K10">
         <v>380</v>
       </c>
-      <c r="I10">
-        <v>380</v>
-      </c>
-      <c r="J10">
-        <v>380</v>
-      </c>
-      <c r="K10">
-        <v>22</v>
-      </c>
       <c r="L10">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>27</v>
+        <v>150</v>
       </c>
       <c r="N10">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="P10">
-        <v>150</v>
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <v>0.5</v>
       </c>
       <c r="S10">
-        <v>50</v>
-      </c>
-      <c r="U10" t="s">
-        <v>3</v>
+        <v>1.5</v>
+      </c>
+      <c r="T10" s="4">
+        <v>1</v>
+      </c>
+      <c r="U10" s="4">
+        <v>25</v>
+      </c>
+      <c r="V10">
+        <v>4</v>
       </c>
       <c r="W10">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="X10">
-        <v>100</v>
-      </c>
-      <c r="Y10">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1167,59 +1160,71 @@
         <v>5230</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1570</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11">
+        <v>19</v>
+      </c>
+      <c r="G11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>23</v>
+      </c>
+      <c r="J11">
+        <v>35</v>
+      </c>
+      <c r="K11">
         <v>380</v>
       </c>
-      <c r="I11">
-        <v>380</v>
-      </c>
-      <c r="J11">
-        <v>380</v>
-      </c>
-      <c r="K11">
-        <v>23</v>
-      </c>
       <c r="L11">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>29</v>
+        <v>150</v>
       </c>
       <c r="N11">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="P11">
-        <v>150</v>
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>0.5</v>
       </c>
       <c r="S11">
-        <v>50</v>
-      </c>
-      <c r="U11" t="s">
+        <v>1.5</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V11">
         <v>4</v>
       </c>
       <c r="W11">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="X11">
         <v>0</v>
       </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1230,59 +1235,72 @@
         <v>6120</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>890</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12">
+        <v>19</v>
+      </c>
+      <c r="G12">
+        <f>2.75*0.8+2.1*0.2</f>
+        <v>2.62</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>26</v>
+      </c>
+      <c r="J12">
+        <v>40</v>
+      </c>
+      <c r="K12">
         <v>320</v>
       </c>
-      <c r="I12">
-        <v>320</v>
-      </c>
-      <c r="J12">
-        <v>320</v>
-      </c>
-      <c r="K12">
-        <v>26</v>
-      </c>
       <c r="L12">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>50</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R12">
+        <v>0.5</v>
+      </c>
+      <c r="S12">
+        <v>1.5</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V12">
+        <v>2</v>
+      </c>
+      <c r="W12">
         <v>100</v>
       </c>
-      <c r="O12">
-        <v>100</v>
-      </c>
-      <c r="P12">
-        <v>100</v>
-      </c>
-      <c r="S12">
-        <v>50</v>
-      </c>
-      <c r="U12" t="s">
-        <v>5</v>
-      </c>
-      <c r="W12">
-        <v>2</v>
-      </c>
       <c r="X12">
-        <v>100</v>
-      </c>
-      <c r="Y12">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1293,59 +1311,71 @@
         <v>6570</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>450</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13">
+        <v>19</v>
+      </c>
+      <c r="G13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>26</v>
+      </c>
+      <c r="J13">
+        <v>40</v>
+      </c>
+      <c r="K13">
         <v>300</v>
       </c>
-      <c r="I13">
-        <v>300</v>
-      </c>
-      <c r="J13">
-        <v>300</v>
-      </c>
-      <c r="K13">
-        <v>26</v>
-      </c>
       <c r="L13">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>50</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13">
+        <v>0.5</v>
+      </c>
+      <c r="S13">
+        <v>1.5</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V13">
+        <v>2</v>
+      </c>
+      <c r="W13">
         <v>100</v>
       </c>
-      <c r="O13">
-        <v>100</v>
-      </c>
-      <c r="P13">
-        <v>100</v>
-      </c>
-      <c r="S13">
-        <v>50</v>
-      </c>
-      <c r="U13" t="s">
-        <v>6</v>
-      </c>
-      <c r="W13">
-        <v>2</v>
-      </c>
       <c r="X13">
-        <v>100</v>
-      </c>
-      <c r="Y13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1356,59 +1386,71 @@
         <v>6900</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>330</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14">
+        <v>19</v>
+      </c>
+      <c r="G14">
+        <v>2.1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>26</v>
+      </c>
+      <c r="J14">
+        <v>40</v>
+      </c>
+      <c r="K14">
         <v>300</v>
       </c>
-      <c r="I14">
-        <v>300</v>
-      </c>
-      <c r="J14">
-        <v>300</v>
-      </c>
-      <c r="K14">
-        <v>26</v>
-      </c>
       <c r="L14">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="N14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="P14">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>7</v>
+      </c>
+      <c r="R14">
+        <v>0.5</v>
       </c>
       <c r="S14">
-        <v>50</v>
-      </c>
-      <c r="U14" t="s">
-        <v>7</v>
+        <v>1.5</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V14">
+        <v>2</v>
       </c>
       <c r="W14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X14">
         <v>0</v>
       </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1419,55 +1461,67 @@
         <v>7200</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15">
+        <v>19</v>
+      </c>
+      <c r="G15">
+        <v>2.1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>26</v>
+      </c>
+      <c r="J15">
+        <v>40</v>
+      </c>
+      <c r="K15" s="1">
         <v>250</v>
       </c>
-      <c r="I15">
-        <v>250</v>
-      </c>
-      <c r="J15">
-        <v>250</v>
-      </c>
-      <c r="K15">
-        <v>33</v>
-      </c>
       <c r="L15">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="N15">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="P15">
-        <v>80</v>
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>8</v>
+      </c>
+      <c r="R15">
+        <v>0.5</v>
       </c>
       <c r="S15">
-        <v>50</v>
-      </c>
-      <c r="U15" t="s">
-        <v>8</v>
+        <v>1.5</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V15">
+        <v>2</v>
       </c>
       <c r="W15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X15">
-        <v>0</v>
-      </c>
-      <c r="Y15">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adattamento per filippine, in attesa di valori sigmaT
</commit_message>
<xml_diff>
--- a/resources/filippine.xlsx
+++ b/resources/filippine.xlsx
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">geo!#REF!</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">geo!$B$3:$C$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,8 +640,8 @@
         <v>19</v>
       </c>
       <c r="G4">
-        <f>2.75*0.8+2.1*0.2</f>
-        <v>2.62</v>
+        <f>(2.75*0.8+2.1*0.2)*9.81</f>
+        <v>25.702200000000001</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -653,7 +653,7 @@
         <v>35</v>
       </c>
       <c r="K4">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -716,8 +716,8 @@
         <v>19</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G6" si="1">2.75*0.8+2.1*0.2</f>
-        <v>2.62</v>
+        <f t="shared" ref="G5:G6" si="1">(2.75*0.8+2.1*0.2)*9.81</f>
+        <v>25.702200000000001</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -729,7 +729,7 @@
         <v>32</v>
       </c>
       <c r="K5">
-        <v>380</v>
+        <v>0.38</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -793,7 +793,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>2.62</v>
+        <v>25.702200000000001</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
@@ -805,7 +805,7 @@
         <v>30</v>
       </c>
       <c r="K6" s="2">
-        <v>400</v>
+        <v>0.4</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -868,7 +868,8 @@
         <v>19</v>
       </c>
       <c r="G7">
-        <v>2.2999999999999998</v>
+        <f>2.3*9.81</f>
+        <v>22.562999999999999</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
@@ -880,7 +881,7 @@
         <v>30</v>
       </c>
       <c r="K7">
-        <v>420</v>
+        <v>0.42</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -943,8 +944,8 @@
         <v>19</v>
       </c>
       <c r="G8">
-        <f>2.75*0.8+2.1*0.2</f>
-        <v>2.62</v>
+        <f>(2.75*0.8+2.1*0.2)*9.81</f>
+        <v>25.702200000000001</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
@@ -956,7 +957,7 @@
         <v>30</v>
       </c>
       <c r="K8">
-        <v>400</v>
+        <v>0.4</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1019,7 +1020,8 @@
         <v>19</v>
       </c>
       <c r="G9">
-        <v>2.2999999999999998</v>
+        <f>2.3*9.81</f>
+        <v>22.562999999999999</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>
@@ -1031,7 +1033,7 @@
         <v>30</v>
       </c>
       <c r="K9">
-        <v>420</v>
+        <v>0.42</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1094,8 +1096,8 @@
         <v>19</v>
       </c>
       <c r="G10">
-        <f>2.75*0.8+2.1*0.2</f>
-        <v>2.62</v>
+        <f>(2.75*0.8+2.1*0.2)*9.81</f>
+        <v>25.702200000000001</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
@@ -1107,7 +1109,7 @@
         <v>32</v>
       </c>
       <c r="K10">
-        <v>380</v>
+        <v>0.38</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1170,7 +1172,8 @@
         <v>19</v>
       </c>
       <c r="G11">
-        <v>2.2999999999999998</v>
+        <f>2.3*9.81</f>
+        <v>22.562999999999999</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
@@ -1182,7 +1185,7 @@
         <v>35</v>
       </c>
       <c r="K11">
-        <v>380</v>
+        <v>0.38</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1245,8 +1248,8 @@
         <v>19</v>
       </c>
       <c r="G12">
-        <f>2.75*0.8+2.1*0.2</f>
-        <v>2.62</v>
+        <f>(2.75*0.8+2.1*0.2)*9.81</f>
+        <v>25.702200000000001</v>
       </c>
       <c r="H12" s="2">
         <v>0</v>
@@ -1258,7 +1261,7 @@
         <v>40</v>
       </c>
       <c r="K12">
-        <v>320</v>
+        <v>0.32</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1321,7 +1324,8 @@
         <v>19</v>
       </c>
       <c r="G13">
-        <v>2.2999999999999998</v>
+        <f>2.3*9.81</f>
+        <v>22.562999999999999</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
@@ -1333,7 +1337,7 @@
         <v>40</v>
       </c>
       <c r="K13">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1396,7 +1400,8 @@
         <v>19</v>
       </c>
       <c r="G14">
-        <v>2.1</v>
+        <f>2.1*9.81</f>
+        <v>20.601000000000003</v>
       </c>
       <c r="H14" s="2">
         <v>0</v>
@@ -1408,7 +1413,7 @@
         <v>40</v>
       </c>
       <c r="K14">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1471,7 +1476,8 @@
         <v>19</v>
       </c>
       <c r="G15">
-        <v>2.1</v>
+        <f>2.1*9.81</f>
+        <v>20.601000000000003</v>
       </c>
       <c r="H15" s="2">
         <v>0</v>
@@ -1483,7 +1489,7 @@
         <v>40</v>
       </c>
       <c r="K15" s="1">
-        <v>250</v>
+        <v>0.25</v>
       </c>
       <c r="L15">
         <v>0</v>

</xml_diff>

<commit_message>
commit consegna - i dati in output non sembrano verosimili
</commit_message>
<xml_diff>
--- a/resources/filippine.xlsx
+++ b/resources/filippine.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>3aU2d</t>
   </si>
@@ -69,15 +69,6 @@
     <t>phimax</t>
   </si>
   <si>
-    <t>UCS_matrix</t>
-  </si>
-  <si>
-    <t>UCS_pebble</t>
-  </si>
-  <si>
-    <t>UCS_clasts</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -136,6 +127,12 @@
   </si>
   <si>
     <t>c_med</t>
+  </si>
+  <si>
+    <t>UCS_min</t>
+  </si>
+  <si>
+    <t>UCS_max</t>
   </si>
 </sst>
 </file>
@@ -469,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X15"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,10 +493,9 @@
     <col min="21" max="21" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1"/>
       <c r="C1"/>
@@ -511,20 +507,20 @@
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
       <c r="N1"/>
       <c r="O1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P1"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
     </row>
-    <row r="2" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -545,9 +541,9 @@
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -556,19 +552,19 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -577,49 +573,46 @@
         <v>12</v>
       </c>
       <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="Q3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="R3" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" t="s">
         <v>34</v>
       </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T3" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" t="s">
-        <v>33</v>
-      </c>
-      <c r="V3" t="s">
-        <v>13</v>
-      </c>
-      <c r="W3" t="s">
-        <v>14</v>
-      </c>
-      <c r="X3" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -637,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G4">
         <f>(2.75*0.8+2.1*0.2)*9.81</f>
@@ -686,16 +679,13 @@
         <v>25</v>
       </c>
       <c r="V4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>100</v>
-      </c>
-      <c r="X4">
-        <v>80</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -713,7 +703,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G5">
         <f t="shared" ref="G5:G6" si="1">(2.75*0.8+2.1*0.2)*9.81</f>
@@ -762,16 +752,13 @@
         <v>25</v>
       </c>
       <c r="V5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W5">
-        <v>100</v>
-      </c>
-      <c r="X5">
-        <v>80</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -789,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
@@ -838,16 +825,13 @@
         <v>25</v>
       </c>
       <c r="V6" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W6" s="2">
-        <v>100</v>
-      </c>
-      <c r="X6" s="2">
-        <v>80</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -865,7 +849,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G7">
         <f>2.3*9.81</f>
@@ -914,16 +898,13 @@
         <v>25</v>
       </c>
       <c r="V7">
-        <v>8</v>
-      </c>
-      <c r="W7">
-        <v>100</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="W7" s="2">
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -941,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G8">
         <f>(2.75*0.8+2.1*0.2)*9.81</f>
@@ -990,16 +971,13 @@
         <v>25</v>
       </c>
       <c r="V8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W8">
-        <v>100</v>
-      </c>
-      <c r="X8">
-        <v>80</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1017,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <f>2.3*9.81</f>
@@ -1066,16 +1044,13 @@
         <v>10</v>
       </c>
       <c r="V9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="W9">
-        <v>100</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1093,7 +1068,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G10">
         <f>(2.75*0.8+2.1*0.2)*9.81</f>
@@ -1142,16 +1117,13 @@
         <v>25</v>
       </c>
       <c r="V10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W10">
-        <v>100</v>
-      </c>
-      <c r="X10">
-        <v>80</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1169,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G11">
         <f>2.3*9.81</f>
@@ -1218,16 +1190,13 @@
         <v>0.1</v>
       </c>
       <c r="V11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W11">
-        <v>100</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1245,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G12">
         <f>(2.75*0.8+2.1*0.2)*9.81</f>
@@ -1294,16 +1263,13 @@
         <v>0.1</v>
       </c>
       <c r="V12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W12">
-        <v>100</v>
-      </c>
-      <c r="X12">
-        <v>80</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1321,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G13">
         <f>2.3*9.81</f>
@@ -1370,16 +1336,13 @@
         <v>0.1</v>
       </c>
       <c r="V13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W13">
-        <v>100</v>
-      </c>
-      <c r="X13">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1397,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G14">
         <f>2.1*9.81</f>
@@ -1446,16 +1409,13 @@
         <v>0.1</v>
       </c>
       <c r="V14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1473,7 +1433,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G15">
         <f>2.1*9.81</f>
@@ -1522,13 +1482,10 @@
         <v>0.1</v>
       </c>
       <c r="V15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiunti coefficienti di efficienza TBM e produzione con distribuzioni triangolari
</commit_message>
<xml_diff>
--- a/resources/filippine.xlsx
+++ b/resources/filippine.xlsx
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">geo!#REF!</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">geo!$B$3:$C$3</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual" refMode="R1C1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>3aU2d</t>
   </si>
@@ -51,9 +51,6 @@
     <t>3bU1b</t>
   </si>
   <si>
-    <t>3cU1b</t>
-  </si>
-  <si>
     <t>3cU1a</t>
   </si>
   <si>
@@ -111,12 +108,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Modulo deformazione</t>
-  </si>
-  <si>
-    <t>Qualità ammasso</t>
-  </si>
-  <si>
     <t>w_inflow_min</t>
   </si>
   <si>
@@ -133,13 +124,103 @@
   </si>
   <si>
     <t>UCS_max</t>
+  </si>
+  <si>
+    <t>open_bould_eff_min</t>
+  </si>
+  <si>
+    <t>open_bould_eff_avg</t>
+  </si>
+  <si>
+    <t>open_bould_eff_max</t>
+  </si>
+  <si>
+    <t>open_water_eff_min</t>
+  </si>
+  <si>
+    <t>open_water_eff_avg</t>
+  </si>
+  <si>
+    <t>open_water_eff_max</t>
+  </si>
+  <si>
+    <t>open_mixit_eff_min</t>
+  </si>
+  <si>
+    <t>open_mixit_eff_avg</t>
+  </si>
+  <si>
+    <t>open_mixit_eff_max</t>
+  </si>
+  <si>
+    <t>open_tbm_eff_min</t>
+  </si>
+  <si>
+    <t>open_tbm_eff_avg</t>
+  </si>
+  <si>
+    <t>open_tbm_eff_max</t>
+  </si>
+  <si>
+    <t>dual_std_eff_min</t>
+  </si>
+  <si>
+    <t>dual_std_eff_avg</t>
+  </si>
+  <si>
+    <t>dual_std_eff_max</t>
+  </si>
+  <si>
+    <t>dual_bould_eff_min</t>
+  </si>
+  <si>
+    <t>dual_bould_eff_avg</t>
+  </si>
+  <si>
+    <t>dual_bould_eff_max</t>
+  </si>
+  <si>
+    <t>dual_water_eff_min</t>
+  </si>
+  <si>
+    <t>dual_water_eff_avg</t>
+  </si>
+  <si>
+    <t>dual_water_eff_max</t>
+  </si>
+  <si>
+    <t>dual_mixit_eff_min</t>
+  </si>
+  <si>
+    <t>dual_mixit_eff_avg</t>
+  </si>
+  <si>
+    <t>dual_mixit_eff_max</t>
+  </si>
+  <si>
+    <t>dual_tbm_eff_min</t>
+  </si>
+  <si>
+    <t>dual_tbm_eff_avg</t>
+  </si>
+  <si>
+    <t>dual_tbm_eff_max</t>
+  </si>
+  <si>
+    <t>open_std_eff_min</t>
+  </si>
+  <si>
+    <t>open_std_eff_avg</t>
+  </si>
+  <si>
+    <t>open_std_eff_max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,19 +234,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -182,10 +265,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -466,37 +549,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:BA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AY20" sqref="AY20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
+    <row r="1" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
@@ -506,22 +622,18 @@
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
-      <c r="K1" t="s">
-        <v>27</v>
-      </c>
+      <c r="K1"/>
       <c r="L1"/>
       <c r="M1"/>
       <c r="N1"/>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
+      <c r="O1"/>
       <c r="P1"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -537,82 +649,172 @@
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="U3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" t="s">
+        <v>30</v>
+      </c>
+      <c r="W3" t="s">
+        <v>31</v>
+      </c>
+      <c r="X3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA3" t="s">
         <v>32</v>
       </c>
-      <c r="N3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" t="s">
-        <v>30</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="AB3" t="s">
         <v>33</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AC3" t="s">
         <v>34</v>
       </c>
+      <c r="AD3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -623,14 +825,14 @@
         <v>290</v>
       </c>
       <c r="D4">
-        <f>C4-B4</f>
+        <f t="shared" ref="D4:D15" si="0">C4-B4</f>
         <v>310</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <f>(2.75*0.8+2.1*0.2)*9.81</f>
@@ -679,13 +881,103 @@
         <v>25</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="W4">
         <v>140</v>
       </c>
+      <c r="X4">
+        <v>0.74</v>
+      </c>
+      <c r="Y4">
+        <v>0.75</v>
+      </c>
+      <c r="Z4">
+        <v>0.76</v>
+      </c>
+      <c r="AA4">
+        <v>0.15</v>
+      </c>
+      <c r="AB4">
+        <v>0.2</v>
+      </c>
+      <c r="AC4">
+        <v>0.22</v>
+      </c>
+      <c r="AD4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AE4">
+        <v>0.15</v>
+      </c>
+      <c r="AF4">
+        <v>0.25</v>
+      </c>
+      <c r="AG4">
+        <v>0.1</v>
+      </c>
+      <c r="AH4">
+        <v>0.1</v>
+      </c>
+      <c r="AI4">
+        <v>0.1</v>
+      </c>
+      <c r="AJ4">
+        <v>0.7</v>
+      </c>
+      <c r="AK4">
+        <v>0.7</v>
+      </c>
+      <c r="AL4">
+        <v>0.7</v>
+      </c>
+      <c r="AM4">
+        <v>0.75</v>
+      </c>
+      <c r="AN4">
+        <v>0.75</v>
+      </c>
+      <c r="AO4">
+        <v>0.75</v>
+      </c>
+      <c r="AP4">
+        <v>0.1</v>
+      </c>
+      <c r="AQ4">
+        <v>0.12</v>
+      </c>
+      <c r="AR4">
+        <v>0.15</v>
+      </c>
+      <c r="AS4">
+        <v>0.05</v>
+      </c>
+      <c r="AT4">
+        <v>0.05</v>
+      </c>
+      <c r="AU4">
+        <v>0.05</v>
+      </c>
+      <c r="AV4">
+        <v>0.05</v>
+      </c>
+      <c r="AW4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX4">
+        <v>0.1</v>
+      </c>
+      <c r="AY4">
+        <v>0.7</v>
+      </c>
+      <c r="AZ4">
+        <v>0.7</v>
+      </c>
+      <c r="BA4">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -696,17 +988,17 @@
         <v>510</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5" si="0">C5-B5</f>
+        <f t="shared" si="0"/>
         <v>220</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G6" si="1">(2.75*0.8+2.1*0.2)*9.81</f>
+        <f>(2.75*0.8+2.1*0.2)*9.81</f>
         <v>25.702200000000001</v>
       </c>
       <c r="H5">
@@ -752,52 +1044,142 @@
         <v>25</v>
       </c>
       <c r="V5">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="W5">
         <v>140</v>
       </c>
+      <c r="X5">
+        <v>0.74</v>
+      </c>
+      <c r="Y5">
+        <v>0.75</v>
+      </c>
+      <c r="Z5">
+        <v>0.76</v>
+      </c>
+      <c r="AA5">
+        <v>0.15</v>
+      </c>
+      <c r="AB5">
+        <v>0.2</v>
+      </c>
+      <c r="AC5">
+        <v>0.22</v>
+      </c>
+      <c r="AD5">
+        <v>0.19</v>
+      </c>
+      <c r="AE5">
+        <v>0.2</v>
+      </c>
+      <c r="AF5">
+        <v>0.25</v>
+      </c>
+      <c r="AG5">
+        <v>0.1</v>
+      </c>
+      <c r="AH5">
+        <v>0.1</v>
+      </c>
+      <c r="AI5">
+        <v>0.1</v>
+      </c>
+      <c r="AJ5">
+        <v>0.7</v>
+      </c>
+      <c r="AK5">
+        <v>0.7</v>
+      </c>
+      <c r="AL5">
+        <v>0.7</v>
+      </c>
+      <c r="AM5">
+        <v>0.75</v>
+      </c>
+      <c r="AN5">
+        <v>0.75</v>
+      </c>
+      <c r="AO5">
+        <v>0.75</v>
+      </c>
+      <c r="AP5">
+        <v>0.1</v>
+      </c>
+      <c r="AQ5">
+        <v>0.12</v>
+      </c>
+      <c r="AR5">
+        <v>0.15</v>
+      </c>
+      <c r="AS5">
+        <v>0.1</v>
+      </c>
+      <c r="AT5">
+        <v>0.1</v>
+      </c>
+      <c r="AU5">
+        <v>0.1</v>
+      </c>
+      <c r="AV5">
+        <v>0.05</v>
+      </c>
+      <c r="AW5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX5">
+        <v>0.1</v>
+      </c>
+      <c r="AY5">
+        <v>0.7</v>
+      </c>
+      <c r="AZ5">
+        <v>0.7</v>
+      </c>
+      <c r="BA5">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>510</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>1090</v>
       </c>
-      <c r="D6" s="2">
-        <f t="shared" ref="D6:D15" si="2">C6-B6</f>
+      <c r="D6">
+        <f t="shared" si="0"/>
         <v>580</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>16</v>
+      <c r="F6" t="s">
+        <v>15</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f>(2.75*0.8+2.1*0.2)*9.81</f>
         <v>25.702200000000001</v>
       </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>21</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>30</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <v>0.4</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6">
         <v>180</v>
       </c>
       <c r="N6">
@@ -809,7 +1191,7 @@
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" t="s">
         <v>1</v>
       </c>
       <c r="R6">
@@ -824,14 +1206,104 @@
       <c r="U6">
         <v>25</v>
       </c>
-      <c r="V6" s="2">
-        <v>1</v>
-      </c>
-      <c r="W6" s="2">
+      <c r="V6">
+        <v>139</v>
+      </c>
+      <c r="W6">
         <v>140</v>
       </c>
+      <c r="X6">
+        <v>0.74</v>
+      </c>
+      <c r="Y6">
+        <v>0.75</v>
+      </c>
+      <c r="Z6">
+        <v>0.76</v>
+      </c>
+      <c r="AA6">
+        <v>0.15</v>
+      </c>
+      <c r="AB6">
+        <v>0.2</v>
+      </c>
+      <c r="AC6">
+        <v>0.22</v>
+      </c>
+      <c r="AD6">
+        <v>0.19</v>
+      </c>
+      <c r="AE6">
+        <v>0.2</v>
+      </c>
+      <c r="AF6">
+        <v>0.25</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AH6">
+        <v>0.1</v>
+      </c>
+      <c r="AI6">
+        <v>0.15</v>
+      </c>
+      <c r="AJ6">
+        <v>0.7</v>
+      </c>
+      <c r="AK6">
+        <v>0.7</v>
+      </c>
+      <c r="AL6">
+        <v>0.7</v>
+      </c>
+      <c r="AM6">
+        <v>0.75</v>
+      </c>
+      <c r="AN6">
+        <v>0.75</v>
+      </c>
+      <c r="AO6">
+        <v>0.75</v>
+      </c>
+      <c r="AP6">
+        <v>0.1</v>
+      </c>
+      <c r="AQ6">
+        <v>0.12</v>
+      </c>
+      <c r="AR6">
+        <v>0.15</v>
+      </c>
+      <c r="AS6">
+        <v>0.1</v>
+      </c>
+      <c r="AT6">
+        <v>0.1</v>
+      </c>
+      <c r="AU6">
+        <v>0.1</v>
+      </c>
+      <c r="AV6">
+        <v>0.05</v>
+      </c>
+      <c r="AW6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX6">
+        <v>0.1</v>
+      </c>
+      <c r="AY6">
+        <v>0.7</v>
+      </c>
+      <c r="AZ6">
+        <v>0.7</v>
+      </c>
+      <c r="BA6">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -842,20 +1314,20 @@
         <v>1690</v>
       </c>
       <c r="D7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <f>2.3*9.81</f>
         <v>22.562999999999999</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
@@ -900,11 +1372,101 @@
       <c r="V7">
         <v>1</v>
       </c>
-      <c r="W7" s="2">
+      <c r="W7">
         <v>10</v>
       </c>
+      <c r="X7">
+        <v>0.74</v>
+      </c>
+      <c r="Y7">
+        <v>0.75</v>
+      </c>
+      <c r="Z7">
+        <v>0.76</v>
+      </c>
+      <c r="AA7">
+        <v>0.19</v>
+      </c>
+      <c r="AB7">
+        <v>0.2</v>
+      </c>
+      <c r="AC7">
+        <v>0.22</v>
+      </c>
+      <c r="AD7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AE7">
+        <v>0.15</v>
+      </c>
+      <c r="AF7">
+        <v>0.2</v>
+      </c>
+      <c r="AG7">
+        <v>0.2</v>
+      </c>
+      <c r="AH7">
+        <v>0.2</v>
+      </c>
+      <c r="AI7">
+        <v>0.2</v>
+      </c>
+      <c r="AJ7">
+        <v>0.7</v>
+      </c>
+      <c r="AK7">
+        <v>0.7</v>
+      </c>
+      <c r="AL7">
+        <v>0.7</v>
+      </c>
+      <c r="AM7">
+        <v>0.7</v>
+      </c>
+      <c r="AN7">
+        <v>0.75</v>
+      </c>
+      <c r="AO7">
+        <v>0.75</v>
+      </c>
+      <c r="AP7">
+        <v>0.15</v>
+      </c>
+      <c r="AQ7">
+        <v>0.18</v>
+      </c>
+      <c r="AR7">
+        <v>0.2</v>
+      </c>
+      <c r="AS7">
+        <v>0.1</v>
+      </c>
+      <c r="AT7">
+        <v>0.1</v>
+      </c>
+      <c r="AU7">
+        <v>0.1</v>
+      </c>
+      <c r="AV7">
+        <v>0.1</v>
+      </c>
+      <c r="AW7">
+        <v>0.12</v>
+      </c>
+      <c r="AX7">
+        <v>0.15</v>
+      </c>
+      <c r="AY7">
+        <v>0.7</v>
+      </c>
+      <c r="AZ7">
+        <v>0.7</v>
+      </c>
+      <c r="BA7">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -915,20 +1477,20 @@
         <v>2550</v>
       </c>
       <c r="D8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>860</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8">
         <f>(2.75*0.8+2.1*0.2)*9.81</f>
         <v>25.702200000000001</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
@@ -971,13 +1533,103 @@
         <v>25</v>
       </c>
       <c r="V8">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="W8">
         <v>140</v>
       </c>
+      <c r="X8">
+        <v>0.74</v>
+      </c>
+      <c r="Y8">
+        <v>0.75</v>
+      </c>
+      <c r="Z8">
+        <v>0.76</v>
+      </c>
+      <c r="AA8">
+        <v>0.15</v>
+      </c>
+      <c r="AB8">
+        <v>0.2</v>
+      </c>
+      <c r="AC8">
+        <v>0.22</v>
+      </c>
+      <c r="AD8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AE8">
+        <v>0.15</v>
+      </c>
+      <c r="AF8">
+        <v>0.2</v>
+      </c>
+      <c r="AG8">
+        <v>0.2</v>
+      </c>
+      <c r="AH8">
+        <v>0.1</v>
+      </c>
+      <c r="AI8">
+        <v>0.1</v>
+      </c>
+      <c r="AJ8">
+        <v>0.75</v>
+      </c>
+      <c r="AK8">
+        <v>0.75</v>
+      </c>
+      <c r="AL8">
+        <v>0.75</v>
+      </c>
+      <c r="AM8">
+        <v>0.65</v>
+      </c>
+      <c r="AN8">
+        <v>0.7</v>
+      </c>
+      <c r="AO8">
+        <v>0.75</v>
+      </c>
+      <c r="AP8">
+        <v>0.1</v>
+      </c>
+      <c r="AQ8">
+        <v>0.12</v>
+      </c>
+      <c r="AR8">
+        <v>0.15</v>
+      </c>
+      <c r="AS8">
+        <v>0.1</v>
+      </c>
+      <c r="AT8">
+        <v>0.1</v>
+      </c>
+      <c r="AU8">
+        <v>0.1</v>
+      </c>
+      <c r="AV8">
+        <v>0.05</v>
+      </c>
+      <c r="AW8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX8">
+        <v>0.1</v>
+      </c>
+      <c r="AY8">
+        <v>0.65</v>
+      </c>
+      <c r="AZ8">
+        <v>0.7</v>
+      </c>
+      <c r="BA8">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -988,20 +1640,20 @@
         <v>3140</v>
       </c>
       <c r="D9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>590</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <f>2.3*9.81</f>
         <v>22.562999999999999</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
@@ -1049,8 +1701,98 @@
       <c r="W9">
         <v>10</v>
       </c>
+      <c r="X9">
+        <v>0.74</v>
+      </c>
+      <c r="Y9">
+        <v>0.75</v>
+      </c>
+      <c r="Z9">
+        <v>0.76</v>
+      </c>
+      <c r="AA9">
+        <v>0.19</v>
+      </c>
+      <c r="AB9">
+        <v>0.2</v>
+      </c>
+      <c r="AC9">
+        <v>0.22</v>
+      </c>
+      <c r="AD9">
+        <v>0.04</v>
+      </c>
+      <c r="AE9">
+        <v>0.05</v>
+      </c>
+      <c r="AF9">
+        <v>0.1</v>
+      </c>
+      <c r="AG9">
+        <v>0.19</v>
+      </c>
+      <c r="AH9">
+        <v>0.2</v>
+      </c>
+      <c r="AI9">
+        <v>0.25</v>
+      </c>
+      <c r="AJ9">
+        <v>0.75</v>
+      </c>
+      <c r="AK9">
+        <v>0.75</v>
+      </c>
+      <c r="AL9">
+        <v>0.75</v>
+      </c>
+      <c r="AM9">
+        <v>0.6</v>
+      </c>
+      <c r="AN9">
+        <v>0.65</v>
+      </c>
+      <c r="AO9">
+        <v>0.7</v>
+      </c>
+      <c r="AP9">
+        <v>0.15</v>
+      </c>
+      <c r="AQ9">
+        <v>0.18</v>
+      </c>
+      <c r="AR9">
+        <v>0.2</v>
+      </c>
+      <c r="AS9">
+        <v>0.05</v>
+      </c>
+      <c r="AT9">
+        <v>0.05</v>
+      </c>
+      <c r="AU9">
+        <v>0.05</v>
+      </c>
+      <c r="AV9">
+        <v>0.1</v>
+      </c>
+      <c r="AW9">
+        <v>0.12</v>
+      </c>
+      <c r="AX9">
+        <v>0.15</v>
+      </c>
+      <c r="AY9">
+        <v>0.65</v>
+      </c>
+      <c r="AZ9">
+        <v>0.65</v>
+      </c>
+      <c r="BA9">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1061,20 +1803,20 @@
         <v>3660</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>520</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10">
         <f>(2.75*0.8+2.1*0.2)*9.81</f>
         <v>25.702200000000001</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
@@ -1110,20 +1852,110 @@
       <c r="S10">
         <v>1.5</v>
       </c>
-      <c r="T10" s="4">
+      <c r="T10">
         <v>1</v>
       </c>
-      <c r="U10" s="4">
+      <c r="U10">
         <v>25</v>
       </c>
       <c r="V10">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="W10">
         <v>140</v>
       </c>
+      <c r="X10">
+        <v>0.74</v>
+      </c>
+      <c r="Y10">
+        <v>0.75</v>
+      </c>
+      <c r="Z10">
+        <v>0.76</v>
+      </c>
+      <c r="AA10">
+        <v>0.15</v>
+      </c>
+      <c r="AB10">
+        <v>0.2</v>
+      </c>
+      <c r="AC10">
+        <v>0.22</v>
+      </c>
+      <c r="AD10">
+        <v>0.04</v>
+      </c>
+      <c r="AE10">
+        <v>0.05</v>
+      </c>
+      <c r="AF10">
+        <v>0.05</v>
+      </c>
+      <c r="AG10">
+        <v>0.1</v>
+      </c>
+      <c r="AH10">
+        <v>0.15</v>
+      </c>
+      <c r="AI10">
+        <v>0.2</v>
+      </c>
+      <c r="AJ10">
+        <v>0.75</v>
+      </c>
+      <c r="AK10">
+        <v>0.75</v>
+      </c>
+      <c r="AL10">
+        <v>0.75</v>
+      </c>
+      <c r="AM10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AN10">
+        <v>0.6</v>
+      </c>
+      <c r="AO10">
+        <v>0.65</v>
+      </c>
+      <c r="AP10">
+        <v>0.1</v>
+      </c>
+      <c r="AQ10">
+        <v>0.12</v>
+      </c>
+      <c r="AR10">
+        <v>0.15</v>
+      </c>
+      <c r="AS10">
+        <v>0.05</v>
+      </c>
+      <c r="AT10">
+        <v>0.05</v>
+      </c>
+      <c r="AU10">
+        <v>0.05</v>
+      </c>
+      <c r="AV10">
+        <v>0.05</v>
+      </c>
+      <c r="AW10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX10">
+        <v>0.1</v>
+      </c>
+      <c r="AY10">
+        <v>0.6</v>
+      </c>
+      <c r="AZ10">
+        <v>0.65</v>
+      </c>
+      <c r="BA10">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1134,20 +1966,20 @@
         <v>5230</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1570</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11">
         <f>2.3*9.81</f>
         <v>22.562999999999999</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
@@ -1186,7 +2018,7 @@
       <c r="T11">
         <v>0</v>
       </c>
-      <c r="U11" s="1">
+      <c r="U11">
         <v>0.1</v>
       </c>
       <c r="V11">
@@ -1195,8 +2027,98 @@
       <c r="W11">
         <v>10</v>
       </c>
+      <c r="X11">
+        <v>0.74</v>
+      </c>
+      <c r="Y11">
+        <v>0.75</v>
+      </c>
+      <c r="Z11">
+        <v>0.76</v>
+      </c>
+      <c r="AA11">
+        <v>0.19</v>
+      </c>
+      <c r="AB11">
+        <v>0.2</v>
+      </c>
+      <c r="AC11">
+        <v>0.22</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0.19</v>
+      </c>
+      <c r="AH11">
+        <v>0.2</v>
+      </c>
+      <c r="AI11">
+        <v>0.21</v>
+      </c>
+      <c r="AJ11">
+        <v>0.75</v>
+      </c>
+      <c r="AK11">
+        <v>0.75</v>
+      </c>
+      <c r="AL11">
+        <v>0.75</v>
+      </c>
+      <c r="AM11">
+        <v>0.75</v>
+      </c>
+      <c r="AN11">
+        <v>0.75</v>
+      </c>
+      <c r="AO11">
+        <v>0.75</v>
+      </c>
+      <c r="AP11">
+        <v>0.2</v>
+      </c>
+      <c r="AQ11">
+        <v>0.2</v>
+      </c>
+      <c r="AR11">
+        <v>0.22</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
+        <v>0.2</v>
+      </c>
+      <c r="AW11">
+        <v>0.2</v>
+      </c>
+      <c r="AX11">
+        <v>0.2</v>
+      </c>
+      <c r="AY11">
+        <v>0.75</v>
+      </c>
+      <c r="AZ11">
+        <v>0.75</v>
+      </c>
+      <c r="BA11">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1207,20 +2129,20 @@
         <v>6120</v>
       </c>
       <c r="D12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>890</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12">
         <f>(2.75*0.8+2.1*0.2)*9.81</f>
         <v>25.702200000000001</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
@@ -1259,17 +2181,107 @@
       <c r="T12">
         <v>0</v>
       </c>
-      <c r="U12" s="1">
+      <c r="U12">
         <v>0.1</v>
       </c>
       <c r="V12">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="W12">
         <v>140</v>
       </c>
+      <c r="X12">
+        <v>0.69</v>
+      </c>
+      <c r="Y12">
+        <v>0.7</v>
+      </c>
+      <c r="Z12">
+        <v>0.71</v>
+      </c>
+      <c r="AA12">
+        <v>0.15</v>
+      </c>
+      <c r="AB12">
+        <v>0.2</v>
+      </c>
+      <c r="AC12">
+        <v>0.22</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0.15</v>
+      </c>
+      <c r="AH12">
+        <v>0.2</v>
+      </c>
+      <c r="AI12">
+        <v>0.21</v>
+      </c>
+      <c r="AJ12">
+        <v>0.7</v>
+      </c>
+      <c r="AK12">
+        <v>0.75</v>
+      </c>
+      <c r="AL12">
+        <v>0.75</v>
+      </c>
+      <c r="AM12">
+        <v>0.7</v>
+      </c>
+      <c r="AN12">
+        <v>0.7</v>
+      </c>
+      <c r="AO12">
+        <v>0.7</v>
+      </c>
+      <c r="AP12">
+        <v>0.15</v>
+      </c>
+      <c r="AQ12">
+        <v>0.2</v>
+      </c>
+      <c r="AR12">
+        <v>0.22</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12">
+        <v>0</v>
+      </c>
+      <c r="AU12">
+        <v>0</v>
+      </c>
+      <c r="AV12">
+        <v>0.15</v>
+      </c>
+      <c r="AW12">
+        <v>0.2</v>
+      </c>
+      <c r="AX12">
+        <v>0.2</v>
+      </c>
+      <c r="AY12">
+        <v>0.7</v>
+      </c>
+      <c r="AZ12">
+        <v>0.75</v>
+      </c>
+      <c r="BA12">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1277,23 +2289,23 @@
         <v>6120</v>
       </c>
       <c r="C13">
-        <v>6570</v>
+        <v>6900</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
-        <v>450</v>
+        <f t="shared" si="0"/>
+        <v>780</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13">
         <f>2.3*9.81</f>
         <v>22.562999999999999</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
@@ -1332,7 +2344,7 @@
       <c r="T13">
         <v>0</v>
       </c>
-      <c r="U13" s="1">
+      <c r="U13">
         <v>0.1</v>
       </c>
       <c r="V13">
@@ -1341,32 +2353,122 @@
       <c r="W13">
         <v>10</v>
       </c>
+      <c r="X13">
+        <v>0.6</v>
+      </c>
+      <c r="Y13">
+        <v>0.6</v>
+      </c>
+      <c r="Z13">
+        <v>0.65</v>
+      </c>
+      <c r="AA13">
+        <v>0.2</v>
+      </c>
+      <c r="AB13">
+        <v>0.22</v>
+      </c>
+      <c r="AC13">
+        <v>0.25</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <v>0.19</v>
+      </c>
+      <c r="AH13">
+        <v>0.2</v>
+      </c>
+      <c r="AI13">
+        <v>0.21</v>
+      </c>
+      <c r="AJ13">
+        <v>0.65</v>
+      </c>
+      <c r="AK13">
+        <v>0.7</v>
+      </c>
+      <c r="AL13">
+        <v>0.7</v>
+      </c>
+      <c r="AM13">
+        <v>0.6</v>
+      </c>
+      <c r="AN13">
+        <v>0.6</v>
+      </c>
+      <c r="AO13">
+        <v>0.65</v>
+      </c>
+      <c r="AP13">
+        <v>0.2</v>
+      </c>
+      <c r="AQ13">
+        <v>0.22</v>
+      </c>
+      <c r="AR13">
+        <v>0.25</v>
+      </c>
+      <c r="AS13">
+        <v>0</v>
+      </c>
+      <c r="AT13">
+        <v>0</v>
+      </c>
+      <c r="AU13">
+        <v>0</v>
+      </c>
+      <c r="AV13">
+        <v>0.2</v>
+      </c>
+      <c r="AW13">
+        <v>0.2</v>
+      </c>
+      <c r="AX13">
+        <v>0.2</v>
+      </c>
+      <c r="AY13">
+        <v>0.65</v>
+      </c>
+      <c r="AZ13">
+        <v>0.7</v>
+      </c>
+      <c r="BA13">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14">
-        <v>6570</v>
+        <v>6900</v>
       </c>
       <c r="C14">
-        <v>6900</v>
+        <v>7000</v>
       </c>
       <c r="D14">
-        <f t="shared" si="2"/>
-        <v>330</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <f>2.1*9.81</f>
         <v>20.601000000000003</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
@@ -1405,7 +2507,7 @@
       <c r="T14">
         <v>0</v>
       </c>
-      <c r="U14" s="1">
+      <c r="U14">
         <v>0.1</v>
       </c>
       <c r="V14">
@@ -1414,32 +2516,122 @@
       <c r="W14">
         <v>10</v>
       </c>
+      <c r="X14">
+        <v>0.54</v>
+      </c>
+      <c r="Y14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Z14">
+        <v>0.6</v>
+      </c>
+      <c r="AA14">
+        <v>0.24</v>
+      </c>
+      <c r="AB14">
+        <v>0.25</v>
+      </c>
+      <c r="AC14">
+        <v>0.3</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AK14">
+        <v>0.6</v>
+      </c>
+      <c r="AL14">
+        <v>0.6</v>
+      </c>
+      <c r="AM14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AN14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AO14">
+        <v>0.6</v>
+      </c>
+      <c r="AP14">
+        <v>0.25</v>
+      </c>
+      <c r="AQ14">
+        <v>0.25</v>
+      </c>
+      <c r="AR14">
+        <v>0.3</v>
+      </c>
+      <c r="AS14">
+        <v>0</v>
+      </c>
+      <c r="AT14">
+        <v>0</v>
+      </c>
+      <c r="AU14">
+        <v>0</v>
+      </c>
+      <c r="AV14">
+        <v>0</v>
+      </c>
+      <c r="AW14">
+        <v>0</v>
+      </c>
+      <c r="AX14">
+        <v>0</v>
+      </c>
+      <c r="AY14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AZ14">
+        <v>0.6</v>
+      </c>
+      <c r="BA14">
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="B15">
-        <v>6900</v>
+        <v>7000</v>
       </c>
       <c r="C15">
         <v>7200</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
-        <v>300</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15">
         <f>2.1*9.81</f>
         <v>20.601000000000003</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
@@ -1448,7 +2640,7 @@
       <c r="J15">
         <v>40</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15">
         <v>0.25</v>
       </c>
       <c r="L15">
@@ -1467,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="Q15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R15">
         <v>0.5</v>
@@ -1478,7 +2670,7 @@
       <c r="T15">
         <v>0</v>
       </c>
-      <c r="U15" s="1">
+      <c r="U15">
         <v>0.1</v>
       </c>
       <c r="V15">
@@ -1487,8 +2679,107 @@
       <c r="W15">
         <v>10</v>
       </c>
+      <c r="X15">
+        <v>0.49</v>
+      </c>
+      <c r="Y15">
+        <v>0.5</v>
+      </c>
+      <c r="Z15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AA15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AB15">
+        <v>0.3</v>
+      </c>
+      <c r="AC15">
+        <v>0.35</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <v>0.5</v>
+      </c>
+      <c r="AK15">
+        <v>0.5</v>
+      </c>
+      <c r="AL15">
+        <v>0.5</v>
+      </c>
+      <c r="AM15">
+        <v>0.5</v>
+      </c>
+      <c r="AN15">
+        <v>0.5</v>
+      </c>
+      <c r="AO15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AP15">
+        <v>0.3</v>
+      </c>
+      <c r="AQ15">
+        <v>0.3</v>
+      </c>
+      <c r="AR15">
+        <v>0.35</v>
+      </c>
+      <c r="AS15">
+        <v>0</v>
+      </c>
+      <c r="AT15">
+        <v>0</v>
+      </c>
+      <c r="AU15">
+        <v>0</v>
+      </c>
+      <c r="AV15">
+        <v>0</v>
+      </c>
+      <c r="AW15">
+        <v>0</v>
+      </c>
+      <c r="AX15">
+        <v>0</v>
+      </c>
+      <c r="AY15">
+        <v>0.5</v>
+      </c>
+      <c r="AZ15">
+        <v>0.5</v>
+      </c>
+      <c r="BA15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="19:51" x14ac:dyDescent="0.25">
+      <c r="AY20" s="4"/>
+    </row>
+    <row r="23" spans="19:51" x14ac:dyDescent="0.25">
+      <c r="S23" s="3"/>
     </row>
   </sheetData>
+  <sortState ref="A4:BA15">
+    <sortCondition ref="A4:A15"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aggiunto attrito di trascinamento
</commit_message>
<xml_diff>
--- a/resources/filippine.xlsx
+++ b/resources/filippine.xlsx
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AY20" sqref="AY20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,10 +848,12 @@
         <v>35</v>
       </c>
       <c r="K4">
-        <v>0.3</v>
+        <f>(0.3+50)/2</f>
+        <v>25.15</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <f>(50-K4)/2</f>
+        <v>12.425000000000001</v>
       </c>
       <c r="M4">
         <v>120</v>
@@ -1011,10 +1013,12 @@
         <v>32</v>
       </c>
       <c r="K5">
-        <v>0.38</v>
+        <f>(0.38+50)/2</f>
+        <v>25.19</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <f>(50-K5)/2</f>
+        <v>12.404999999999999</v>
       </c>
       <c r="M5">
         <v>150</v>
@@ -1173,11 +1177,13 @@
       <c r="J6">
         <v>30</v>
       </c>
-      <c r="K6">
-        <v>0.4</v>
+      <c r="K6" s="1">
+        <f>(0.4+50)/2</f>
+        <v>25.2</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <f t="shared" ref="L6:L12" si="1">(50-K6)/2</f>
+        <v>12.4</v>
       </c>
       <c r="M6">
         <v>180</v>
@@ -1500,10 +1506,12 @@
         <v>30</v>
       </c>
       <c r="K8">
-        <v>0.4</v>
+        <f>(0.4+50)/2</f>
+        <v>25.2</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>12.4</v>
       </c>
       <c r="M8">
         <v>180</v>
@@ -1826,10 +1834,12 @@
         <v>32</v>
       </c>
       <c r="K10">
-        <v>0.38</v>
+        <f>(0.38+50)/2</f>
+        <v>25.19</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>12.404999999999999</v>
       </c>
       <c r="M10">
         <v>150</v>
@@ -2152,10 +2162,12 @@
         <v>40</v>
       </c>
       <c r="K12">
-        <v>0.32</v>
+        <f>(0.32+50)/2</f>
+        <v>25.16</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>12.42</v>
       </c>
       <c r="M12">
         <v>100</v>
@@ -2640,7 +2652,7 @@
       <c r="J15">
         <v>40</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="4">
         <v>0.25</v>
       </c>
       <c r="L15">

</xml_diff>